<commit_message>
Se retiro el guardado manual de boton en el excel y se integro que sea automaticamente
</commit_message>
<xml_diff>
--- a/gastos_diarios.xlsx
+++ b/gastos_diarios.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -480,6 +480,21 @@
         <v>10000</v>
       </c>
     </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>2023-07-22</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>pago de luz</t>
+        </is>
+      </c>
+      <c r="C4" t="n">
+        <v>100000</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Se reparo el bug donde no se mostraba lo datos ya agregados
</commit_message>
<xml_diff>
--- a/gastos_diarios.xlsx
+++ b/gastos_diarios.xlsx
@@ -1,37 +1,72 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26529"/>
   <workbookPr/>
-  <workbookProtection/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\thega\source\repos\contro_de_gastosV2\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3996DAC-7113-4200-A184-2031CDA184E5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView xWindow="768" yWindow="768" windowWidth="17280" windowHeight="8880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames/>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="8">
+  <si>
+    <t>Fecha</t>
+  </si>
+  <si>
+    <t>Descripción</t>
+  </si>
+  <si>
+    <t>Monto</t>
+  </si>
+  <si>
+    <t>2023-07-22</t>
+  </si>
+  <si>
+    <t>juego</t>
+  </si>
+  <si>
+    <t>lol</t>
+  </si>
+  <si>
+    <t>pago de luz</t>
+  </si>
+  <si>
+    <t>2023-04-21</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <color theme="1"/>
-      <sz val="11"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b val="1"/>
+      <b/>
+      <sz val="11"/>
+      <name val="Calibri"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill/>
+      <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -46,93 +81,43 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin"/>
-      <right style="thin"/>
-      <top style="thin"/>
-      <bottom style="thin"/>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="2">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <colors>
-    <indexedColors>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008000"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00808000"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="00C0C0C0"/>
-      <rgbColor rgb="00808080"/>
-      <rgbColor rgb="009999FF"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00FFFFCC"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00660066"/>
-      <rgbColor rgb="00FF8080"/>
-      <rgbColor rgb="000066CC"/>
-      <rgbColor rgb="00CCCCFF"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="0000CCFF"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00CCFFCC"/>
-      <rgbColor rgb="00FFFF99"/>
-      <rgbColor rgb="0099CCFF"/>
-      <rgbColor rgb="00FF99CC"/>
-      <rgbColor rgb="00CC99FF"/>
-      <rgbColor rgb="00FFCC99"/>
-      <rgbColor rgb="003366FF"/>
-      <rgbColor rgb="0033CCCC"/>
-      <rgbColor rgb="0099CC00"/>
-      <rgbColor rgb="00FFCC00"/>
-      <rgbColor rgb="00FF9900"/>
-      <rgbColor rgb="00FF6600"/>
-      <rgbColor rgb="00666699"/>
-      <rgbColor rgb="00969696"/>
-      <rgbColor rgb="00003366"/>
-      <rgbColor rgb="00339966"/>
-      <rgbColor rgb="00003300"/>
-      <rgbColor rgb="00333300"/>
-      <rgbColor rgb="00993300"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00333399"/>
-      <rgbColor rgb="00333333"/>
-    </indexedColors>
-  </colors>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -420,78 +405,72 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:C4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:C5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="22.21875" customWidth="1"/>
+    <col min="2" max="2" width="19.88671875" customWidth="1"/>
+    <col min="3" max="3" width="16.88671875" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1">
-      <c r="A1" s="1" t="inlineStr">
-        <is>
-          <t>Fecha</t>
-        </is>
-      </c>
-      <c r="B1" s="1" t="inlineStr">
-        <is>
-          <t>Descripción</t>
-        </is>
-      </c>
-      <c r="C1" s="1" t="inlineStr">
-        <is>
-          <t>Monto</t>
-        </is>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
       </c>
     </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>2023-07-22</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>juego</t>
-        </is>
-      </c>
-      <c r="C2" t="n">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2">
         <v>10000</v>
       </c>
     </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>2023-07-22</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>lol</t>
-        </is>
-      </c>
-      <c r="C3" t="n">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3">
         <v>10000</v>
       </c>
     </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>2023-07-22</t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>pago de luz</t>
-        </is>
-      </c>
-      <c r="C4" t="n">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4">
+        <v>100000</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C5">
         <v>100000</v>
       </c>
     </row>

</xml_diff>